<commit_message>
Versión 0.0.0.2 de MVP Importación de facturas de servicios con consumos
</commit_message>
<xml_diff>
--- a/ejemplo_facturas.xlsx
+++ b/ejemplo_facturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanv\dev\work\ori_cc_servicios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10310495-B2B6-4D08-906D-CD336CD51329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53C6A47-70F4-48DF-8D4B-2470CCB1C087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{E9083B62-4189-4ECF-AEC8-0F2110B8689F}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">ejemplo_facturas!$A$1:$H$6</definedName>
+    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">ejemplo_facturas!$A$1:$G$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,19 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t>numero_factura</t>
-  </si>
-  <si>
-    <t>codigo_cliente</t>
-  </si>
-  <si>
-    <t>fecha_emision</t>
-  </si>
-  <si>
-    <t>fecha_vencimiento</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>lectura_anterior</t>
   </si>
@@ -68,45 +56,53 @@
     <t>lectura_actual</t>
   </si>
   <si>
-    <t>consumo</t>
-  </si>
-  <si>
     <t>valor_unitario</t>
   </si>
   <si>
-    <t>FAC001</t>
-  </si>
-  <si>
-    <t>CLI001</t>
-  </si>
-  <si>
-    <t>FAC002</t>
-  </si>
-  <si>
-    <t>CLI002</t>
-  </si>
-  <si>
-    <t>FAC003</t>
-  </si>
-  <si>
-    <t>CLI003</t>
-  </si>
-  <si>
-    <t>FAC004</t>
-  </si>
-  <si>
-    <t>FAC005</t>
-  </si>
-  <si>
-    <t>CLI004</t>
+    <t>id_carpeta</t>
+  </si>
+  <si>
+    <t>id_servicio</t>
+  </si>
+  <si>
+    <t>id_predio</t>
+  </si>
+  <si>
+    <t>id_tercero_cliente</t>
+  </si>
+  <si>
+    <t>periodo_inicio_cobro</t>
+  </si>
+  <si>
+    <t>APTO 0201 A</t>
+  </si>
+  <si>
+    <t>APTO 0201 B</t>
+  </si>
+  <si>
+    <t>APTO 0202 A</t>
+  </si>
+  <si>
+    <t>APTO 0203 B</t>
+  </si>
+  <si>
+    <t>APTO 0202 B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -136,15 +132,18 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -170,17 +169,21 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_1" connectionId="1" xr16:uid="{484F2F74-ADB6-424C-8B3C-9C32A0EE9991}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="9">
+  <queryTableRefresh nextId="11" unboundColumnsRight="1">
     <queryTableFields count="8">
       <queryTableField id="1" name="numero_factura" tableColumnId="1"/>
       <queryTableField id="2" name="codigo_cliente" tableColumnId="2"/>
       <queryTableField id="3" name="fecha_emision" tableColumnId="3"/>
       <queryTableField id="4" name="fecha_vencimiento" tableColumnId="4"/>
+      <queryTableField id="9" dataBound="0" tableColumnId="9"/>
       <queryTableField id="5" name="lectura_anterior" tableColumnId="5"/>
       <queryTableField id="6" name="lectura_actual" tableColumnId="6"/>
-      <queryTableField id="7" name="consumo" tableColumnId="7"/>
-      <queryTableField id="8" name="valor_unitario" tableColumnId="8"/>
+      <queryTableField id="10" dataBound="0" tableColumnId="10"/>
     </queryTableFields>
+    <queryTableDeletedFields count="2">
+      <deletedField name="consumo"/>
+      <deletedField name="valor_unitario"/>
+    </queryTableDeletedFields>
   </queryTableRefresh>
 </queryTable>
 </file>
@@ -189,14 +192,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{307E699F-0C02-4EEE-8296-D9BC5CAABB71}" name="ejemplo_facturas" displayName="ejemplo_facturas" ref="A1:H6" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H6" xr:uid="{307E699F-0C02-4EEE-8296-D9BC5CAABB71}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F7BAF84F-BA3F-4F45-B9BC-1A4109608713}" uniqueName="1" name="numero_factura" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{98093313-DE00-41AE-BE02-6D01AF9DB0B9}" uniqueName="2" name="codigo_cliente" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{C5098F97-18FF-414E-B29E-BDF6629DCF98}" uniqueName="3" name="fecha_emision" queryTableFieldId="3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{559A9718-4F8F-48C7-800D-B781E19EB67C}" uniqueName="4" name="fecha_vencimiento" queryTableFieldId="4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F7BAF84F-BA3F-4F45-B9BC-1A4109608713}" uniqueName="1" name="id_carpeta" queryTableFieldId="1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{98093313-DE00-41AE-BE02-6D01AF9DB0B9}" uniqueName="2" name="id_servicio" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{C5098F97-18FF-414E-B29E-BDF6629DCF98}" uniqueName="3" name="id_predio" queryTableFieldId="3" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{559A9718-4F8F-48C7-800D-B781E19EB67C}" uniqueName="4" name="id_tercero_cliente" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{E2E0A197-719C-43A7-AFC0-25662C0A09DD}" uniqueName="9" name="periodo_inicio_cobro" queryTableFieldId="9" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{4036AA89-01B7-469E-AB7D-56107F94BEE7}" uniqueName="5" name="lectura_anterior" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{69872AB8-87BC-4A5C-AACD-8A193FE3C493}" uniqueName="6" name="lectura_actual" queryTableFieldId="6"/>
-    <tableColumn id="7" xr3:uid="{C4AA0E22-CC4F-4353-AF97-4F493C93A6A1}" uniqueName="7" name="consumo" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{36F27935-6FAF-4019-8E33-0B77006705E2}" uniqueName="8" name="valor_unitario" queryTableFieldId="8"/>
+    <tableColumn id="10" xr3:uid="{523BD59F-33A2-47F4-B550-02A79DA2405F}" uniqueName="10" name="valor_unitario" queryTableFieldId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -521,7 +524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAEE3B5-E027-492A-8E63-AF387BE552D4}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
@@ -529,166 +534,166 @@
     <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45306</v>
-      </c>
-      <c r="D2" s="2">
-        <v>45337</v>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2">
+        <v>202509</v>
+      </c>
+      <c r="F2">
         <v>100050</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>115075</v>
       </c>
-      <c r="G2">
-        <v>15025</v>
-      </c>
       <c r="H2">
-        <v>85000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45311</v>
-      </c>
-      <c r="D3" s="2">
-        <v>45342</v>
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3">
+        <v>202509</v>
+      </c>
+      <c r="F3">
         <v>250000</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>275025</v>
       </c>
-      <c r="G3">
-        <v>25025</v>
-      </c>
       <c r="H3">
-        <v>92000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2">
-        <v>45316</v>
-      </c>
-      <c r="D4" s="2">
-        <v>45347</v>
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
       <c r="E4">
+        <v>202509</v>
+      </c>
+      <c r="F4">
         <v>80000</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>95050</v>
       </c>
-      <c r="G4">
-        <v>15050</v>
-      </c>
       <c r="H4">
-        <v>78000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2">
-        <v>45323</v>
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D5" s="2">
-        <v>45352</v>
+        <v>0</v>
       </c>
       <c r="E5">
+        <v>202509</v>
+      </c>
+      <c r="F5">
         <v>115075</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>132025</v>
       </c>
-      <c r="G5">
-        <v>16950</v>
-      </c>
       <c r="H5">
-        <v>85000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2">
-        <v>45327</v>
-      </c>
-      <c r="D6" s="2">
-        <v>45356</v>
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
       </c>
       <c r="E6">
+        <v>202509</v>
+      </c>
+      <c r="F6">
         <v>320000</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>345075</v>
       </c>
-      <c r="G6">
-        <v>25075</v>
-      </c>
       <c r="H6">
-        <v>95000</v>
+        <v>998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>